<commit_message>
develope getData utility , zip file and extract data util
</commit_message>
<xml_diff>
--- a/src/test/java/com/freecrm/xls/A suite.xlsx
+++ b/src/test/java/com/freecrm/xls/A suite.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestCase_A1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>TCID</t>
   </si>
@@ -40,6 +40,90 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Dummy Data1</t>
+  </si>
+  <si>
+    <t>Dummy Data6</t>
+  </si>
+  <si>
+    <t>Dummy Data11</t>
+  </si>
+  <si>
+    <t>Dummy Data16</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Dummy Data2</t>
+  </si>
+  <si>
+    <t>Dummy Data7</t>
+  </si>
+  <si>
+    <t>Dummy Data12</t>
+  </si>
+  <si>
+    <t>Dummy Data17</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Dummy Data3</t>
+  </si>
+  <si>
+    <t>Dummy Data8</t>
+  </si>
+  <si>
+    <t>Dummy Data13</t>
+  </si>
+  <si>
+    <t>Dummy Data18</t>
+  </si>
+  <si>
+    <t>Dummy Data4</t>
+  </si>
+  <si>
+    <t>Dummy Data9</t>
+  </si>
+  <si>
+    <t>Dummy Data15</t>
+  </si>
+  <si>
+    <t>Dummy Data19</t>
+  </si>
+  <si>
+    <t>Dummy Data5</t>
+  </si>
+  <si>
+    <t>Dummy Data10</t>
+  </si>
+  <si>
+    <t>Dummy Data14</t>
+  </si>
+  <si>
+    <t>Dummy Data111</t>
+  </si>
+  <si>
+    <t>Data_A1</t>
+  </si>
+  <si>
+    <t>Data_A2</t>
+  </si>
+  <si>
+    <t>Data_A3</t>
+  </si>
+  <si>
+    <t>Data_A4</t>
   </si>
 </sst>
 </file>
@@ -69,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -92,13 +176,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -446,12 +546,129 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>